<commit_message>
- added constitutents function - fixed lästige print message
</commit_message>
<xml_diff>
--- a/methodology.xlsx
+++ b/methodology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pertl\Desktop\timing_bond_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C8B41D-0C39-42C1-AEFE-106CBFCE2CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BA5B9-6B2F-4F86-BFE8-6FF5D04B4835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>Book Value</t>
-  </si>
-  <si>
-    <t>Yield</t>
   </si>
   <si>
     <t>Amount Outstanding</t>
@@ -380,7 +377,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9426FF54-AE69-47A8-B70A-8EAFBFBE73BA}" name="Table1" displayName="Table1" ref="A2:G30" totalsRowShown="0">
-  <autoFilter ref="A2:G30" xr:uid="{9426FF54-AE69-47A8-B70A-8EAFBFBE73BA}"/>
+  <autoFilter ref="A2:G30" xr:uid="{9426FF54-AE69-47A8-B70A-8EAFBFBE73BA}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="???"/>
+        <filter val="Yes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D6DE61C0-2CBB-4E51-81BF-C27C100C32DE}" name="Name"/>
     <tableColumn id="6" xr3:uid="{E84A74E3-3090-44A0-85C6-2193AEE0C99C}" name="What do I need?"/>
@@ -659,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -693,7 +697,7 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -705,7 +709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -728,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -751,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -799,13 +803,10 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -837,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -860,7 +861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -883,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -906,7 +907,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -969,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -992,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1066,7 +1067,7 @@
         <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
         <v>78</v>
@@ -1081,7 +1082,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1147,12 +1148,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
@@ -1175,10 +1176,10 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
         <v>53</v>
@@ -1195,7 +1196,7 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
         <v>81</v>
@@ -1215,7 +1216,7 @@
         <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
         <v>81</v>
@@ -1235,7 +1236,7 @@
         <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
         <v>81</v>
@@ -1255,7 +1256,7 @@
         <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
         <v>81</v>
@@ -1275,7 +1276,7 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
- added several new factors
</commit_message>
<xml_diff>
--- a/methodology.xlsx
+++ b/methodology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pertl\Desktop\timing_bond_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BA5B9-6B2F-4F86-BFE8-6FF5D04B4835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF70B37-51DB-41C7-AE7E-89C6BC6FBF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>Daily Prices</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>TRACE</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -377,14 +386,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9426FF54-AE69-47A8-B70A-8EAFBFBE73BA}" name="Table1" displayName="Table1" ref="A2:G30" totalsRowShown="0">
-  <autoFilter ref="A2:G30" xr:uid="{9426FF54-AE69-47A8-B70A-8EAFBFBE73BA}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="???"/>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:G30" xr:uid="{9426FF54-AE69-47A8-B70A-8EAFBFBE73BA}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D6DE61C0-2CBB-4E51-81BF-C27C100C32DE}" name="Name"/>
     <tableColumn id="6" xr3:uid="{E84A74E3-3090-44A0-85C6-2193AEE0C99C}" name="What do I need?"/>
@@ -664,7 +666,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -732,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -755,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -786,7 +788,10 @@
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -838,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -861,7 +866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -884,7 +889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -907,7 +912,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -970,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -993,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1039,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1070,7 +1075,10 @@
         <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>94</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1082,7 +1090,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1125,7 +1133,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1136,7 +1144,7 @@
         <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E22" t="s">
         <v>48</v>
@@ -1148,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1159,7 +1167,7 @@
         <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
         <v>51</v>
@@ -1181,6 +1189,9 @@
       <c r="C24" t="s">
         <v>78</v>
       </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
       <c r="E24" t="s">
         <v>53</v>
       </c>
@@ -1201,6 +1212,9 @@
       <c r="C25" t="s">
         <v>81</v>
       </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
       <c r="E25" t="s">
         <v>55</v>
       </c>
@@ -1219,7 +1233,10 @@
         <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>94</v>
       </c>
       <c r="E26" t="s">
         <v>57</v>
@@ -1239,7 +1256,10 @@
         <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
       </c>
       <c r="E27" t="s">
         <v>59</v>
@@ -1259,7 +1279,10 @@
         <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
       </c>
       <c r="E28" t="s">
         <v>61</v>
@@ -1280,6 +1303,9 @@
       </c>
       <c r="C29" t="s">
         <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>92</v>
       </c>
       <c r="E29" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
- Reorganized code folder - Created data backup
</commit_message>
<xml_diff>
--- a/methodology.xlsx
+++ b/methodology.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pertl\Desktop\timing_bond_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF70B37-51DB-41C7-AE7E-89C6BC6FBF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B71C24-F381-4442-8FFB-1B77584F6898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -318,9 +318,6 @@
   </si>
   <si>
     <t>TRACE</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -665,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,7 +788,7 @@
         <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -945,6 +942,9 @@
       <c r="C13" t="s">
         <v>81</v>
       </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
       <c r="E13" t="s">
         <v>26</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -1190,7 +1190,7 @@
         <v>78</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
         <v>53</v>
@@ -1236,7 +1236,7 @@
         <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
         <v>57</v>
@@ -1259,7 +1259,7 @@
         <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
         <v>59</v>
@@ -1282,7 +1282,7 @@
         <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Fixed issue with lags of factor signals.
</commit_message>
<xml_diff>
--- a/methodology.xlsx
+++ b/methodology.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pertl\Desktop\timing_bond_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B71C24-F381-4442-8FFB-1B77584F6898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47E8C42-9E35-43D2-8194-8FA26486F27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="factors" sheetId="1" r:id="rId1"/>
+    <sheet name="timing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="184">
   <si>
     <t>Name</t>
   </si>
@@ -318,13 +319,283 @@
   </si>
   <si>
     <t>TRACE</t>
+  </si>
+  <si>
+    <t>Acronym</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Momentum</t>
+  </si>
+  <si>
+    <t>MOM2</t>
+  </si>
+  <si>
+    <t>MOM3</t>
+  </si>
+  <si>
+    <t>MOM5</t>
+  </si>
+  <si>
+    <t>MOM6</t>
+  </si>
+  <si>
+    <t>MOM7</t>
+  </si>
+  <si>
+    <t>MOM8</t>
+  </si>
+  <si>
+    <t>MOM9</t>
+  </si>
+  <si>
+    <t>MOM10</t>
+  </si>
+  <si>
+    <t>MOM11</t>
+  </si>
+  <si>
+    <t>VOL2</t>
+  </si>
+  <si>
+    <t>VOL3</t>
+  </si>
+  <si>
+    <t>VOL4</t>
+  </si>
+  <si>
+    <t>VOL5</t>
+  </si>
+  <si>
+    <t>VOL6</t>
+  </si>
+  <si>
+    <t>REV1</t>
+  </si>
+  <si>
+    <t>Reversal</t>
+  </si>
+  <si>
+    <t>REV2</t>
+  </si>
+  <si>
+    <t>TSMOM2</t>
+  </si>
+  <si>
+    <t>TSMOM3</t>
+  </si>
+  <si>
+    <t>TSMOM4</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>VAL2</t>
+  </si>
+  <si>
+    <t>VAL3</t>
+  </si>
+  <si>
+    <t>VAL4</t>
+  </si>
+  <si>
+    <t>VAL5</t>
+  </si>
+  <si>
+    <t>VAL6</t>
+  </si>
+  <si>
+    <t>SPREAD1</t>
+  </si>
+  <si>
+    <t>SPREAD2</t>
+  </si>
+  <si>
+    <t>IPS1</t>
+  </si>
+  <si>
+    <t>Related literature</t>
+  </si>
+  <si>
+    <t>Implementation to obtain $w_{i,t}^{j}$ in our paper</t>
+  </si>
+  <si>
+    <t>Gupta and Kelly (2019)</t>
+  </si>
+  <si>
+    <t>Annualized return in month scaled by annualized past return volatility over 3Y, capped at $t\pm2$</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-2$ to $t$, scaled by annualized past return volatility over 3Y, capped at 2</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-5$ to $t$, scaled by annualized past return volatility over 3Y, capped at 2</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-11$ to $t$, scaled by annualized past return volatility over 10Y, capped at ±2</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-3$ to $t$, scaled by annualized past return volatility over 10Y, capped at ±2</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-59$ to $t$, scaled by annualized past return volatility over 10Y, capped at ±2</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-1$ to $t-1$, scaled by annualized past return volatility over 3Y, capped at ±2</t>
+  </si>
+  <si>
+    <t>Annualized average return over the formation period $t-59$ to $t-12$, scaled by annualized past return volatility over 10Y, capped at ±2</t>
+  </si>
+  <si>
+    <t>Ehsani, Linnainmaa (2019)</t>
+  </si>
+  <si>
+    <t>Sign of return in month $t$</t>
+  </si>
+  <si>
+    <t>Sign of cumulative return over months 2 to $t$</t>
+  </si>
+  <si>
+    <t>Sign of cumulative return over months $t-5$ to $t$</t>
+  </si>
+  <si>
+    <t>Sign of cumulative return over months $t-11$ to $t$</t>
+  </si>
+  <si>
+    <t>Moreira and Muir (2017)</t>
+  </si>
+  <si>
+    <t>Inverse of the variance of daily returns in month $t$, scaled by the average of all monthly variances until $t$</t>
+  </si>
+  <si>
+    <t>Inverse of the std. dev. of daily returns in month $t$, scaled by average of all past std. dev. until $t$</t>
+  </si>
+  <si>
+    <t>Inverse of variance of daily returns in month $t$, estimated via AR(1) log variance, scaled by average of all past variances</t>
+  </si>
+  <si>
+    <t>Cederburg, O'Doherty, Wang, Yan (2020)</t>
+  </si>
+  <si>
+    <t>Inverse variance of daily returns in month $t$, multiplied by 22 over trading days, scaled by past average</t>
+  </si>
+  <si>
+    <t>DeMiguel, Utrera, Uppal (2021)</t>
+  </si>
+  <si>
+    <t>Inverse of std. dev. of market returns in month $t$, scaled by historical average</t>
+  </si>
+  <si>
+    <t>Reschenhofer and Zechner (2021)</t>
+  </si>
+  <si>
+    <t>Level of implied volatility (CBOE VIX) in month $t$</t>
+  </si>
+  <si>
+    <t>Level of implied skewness (CBOE SKEW) in month $t$</t>
+  </si>
+  <si>
+    <t>Moskowitz, Ooi, Pedersen (2012)</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-59$ to $t$</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-11$ to $t$</t>
+  </si>
+  <si>
+    <t>Sign of return in month $t$ × 40% / ex-ante volatility (EWMA of squared daily returns)</t>
+  </si>
+  <si>
+    <t>Sign of cumulative return $t-2$ to $t$ × 40% / ex-ante volatility</t>
+  </si>
+  <si>
+    <t>Sign of cumulative return $t-5$ to $t$ × 40% / ex-ante volatility</t>
+  </si>
+  <si>
+    <t>Sign of cumulative return $t-11$ to $t$ × 40% / ex-ante volatility</t>
+  </si>
+  <si>
+    <t>Campbell &amp; Shiller (1988); Cohen et al. (2003); Haddad et al. (2020)</t>
+  </si>
+  <si>
+    <t>BTM spread: log(B/M long - short); signal = spread - expanding mean / std. dev.</t>
+  </si>
+  <si>
+    <t>BTM spread minus 5-year rolling mean, scaled by std. dev.</t>
+  </si>
+  <si>
+    <t>BTM spread (book value Dec last year); signal = spread - expanding mean / std. dev.</t>
+  </si>
+  <si>
+    <t>BTM spread (Dec book); signal = spread - 5yr rolling mean / std. dev.</t>
+  </si>
+  <si>
+    <t>Quarterly book equity over market equity; signal = spread - expanding mean / std. dev.</t>
+  </si>
+  <si>
+    <t>Quarterly book equity over market equity; signal = spread - 5yr rolling mean / std. dev.</t>
+  </si>
+  <si>
+    <t>Characteristic spread</t>
+  </si>
+  <si>
+    <t>Huang, Liu, Ma, Osiol (2011)</t>
+  </si>
+  <si>
+    <t>Characteristic spread = long - short; signal = spread - expanding mean / std. dev.</t>
+  </si>
+  <si>
+    <t>Characteristic spread = long - short; signal = spread - 5yr rolling mean / std. dev.</t>
+  </si>
+  <si>
+    <t>Issuer-purchaser spread</t>
+  </si>
+  <si>
+    <t>Greenwood and Hanson (2012)</t>
+  </si>
+  <si>
+    <t>Diff in avg YoY net issuance: issuers - repurchasers; signal = diff - expanding mean / std. dev.</t>
+  </si>
+  <si>
+    <t>MOM1</t>
+  </si>
+  <si>
+    <t>MOM4</t>
+  </si>
+  <si>
+    <t>MOM12</t>
+  </si>
+  <si>
+    <t>VOL1</t>
+  </si>
+  <si>
+    <t>VOL7</t>
+  </si>
+  <si>
+    <t>TSMOM1</t>
+  </si>
+  <si>
+    <t>VAL1</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Able</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +610,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Google Sans Text"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -361,14 +638,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Google Sans Text"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -392,6 +695,20 @@
     <tableColumn id="2" xr3:uid="{A7CCD85D-E9F3-45F4-BE8C-DA2B43EDA3C6}" name="Description"/>
     <tableColumn id="3" xr3:uid="{13C2E9BC-F9BE-493A-9B4D-04D8A25AADCC}" name="Cite"/>
     <tableColumn id="4" xr3:uid="{A55AE291-1075-43CE-A0EC-F9F5CBFBC154}" name="Direction"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1D9005A-3701-44A8-A6C8-6D65169F7692}" name="Table2" displayName="Table2" ref="A1:E35" totalsRowShown="0">
+  <autoFilter ref="A1:E35" xr:uid="{F1D9005A-3701-44A8-A6C8-6D65169F7692}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{EF71E0ED-69AD-45B5-B3CB-1A130C8F904B}" name="Acronym" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{87D7EB89-70BE-465C-A2D1-9206C6B2A627}" name="Category"/>
+    <tableColumn id="5" xr3:uid="{B5C95ED8-8AAB-42B1-8D0B-CF486C58FBBE}" name="Status"/>
+    <tableColumn id="3" xr3:uid="{0463E492-FDDE-44D1-8B1C-5293993D783E}" name="Related literature"/>
+    <tableColumn id="4" xr3:uid="{CBCA4ACC-65D6-446C-97C1-C9B4E3F2A51C}" name="Implementation to obtain $w_{i,t}^{j}$ in our paper"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -662,11 +979,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
@@ -677,7 +994,7 @@
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -685,7 +1002,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -708,7 +1025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -731,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -754,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -777,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -800,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -820,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -840,7 +1157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -863,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -886,7 +1203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -909,7 +1226,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -932,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -955,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -975,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -998,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1021,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1044,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1067,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1090,7 +1407,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1113,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1133,7 +1450,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1156,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -1179,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1202,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1225,7 +1542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1248,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -1271,7 +1588,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>73</v>
       </c>
@@ -1294,7 +1611,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1317,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1336,6 +1653,631 @@
       <c r="G30">
         <v>1</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1752AB43-D4D0-4055-B83C-18A0D13E7988}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="57.5546875" customWidth="1"/>
+    <col min="5" max="5" width="111.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A27" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A28" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A30" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A32" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" t="s">
+        <v>167</v>
+      </c>
+      <c r="C33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A34" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19.2" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created simple correlation plot among signals
</commit_message>
<xml_diff>
--- a/methodology.xlsx
+++ b/methodology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pertl\Desktop\timing_bond_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB1968C-7203-4AEC-8A6F-5B215556CB50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3111C23F-F31E-4210-BC41-F4374E4B5C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="220">
   <si>
     <t>Name</t>
   </si>
@@ -622,16 +622,82 @@
     <t>Sign of cumulative return over months $t-3$ to $t$</t>
   </si>
   <si>
-    <t>mom1 scaled by 3Y past return volatility</t>
-  </si>
-  <si>
-    <t>mom3 scaled by 3Y past return volatility</t>
-  </si>
-  <si>
-    <t>mom6 scaled by 3Y past return volatility</t>
-  </si>
-  <si>
     <t>mom12 scaled by 3Y past return volatility</t>
+  </si>
+  <si>
+    <t>vol1</t>
+  </si>
+  <si>
+    <t>vol2</t>
+  </si>
+  <si>
+    <t>vol3</t>
+  </si>
+  <si>
+    <t>vol4</t>
+  </si>
+  <si>
+    <t>Pertl (2025)</t>
+  </si>
+  <si>
+    <t>Inverse rolling 12-month vola, scaled by 12-month average</t>
+  </si>
+  <si>
+    <t>Inverse rolling 12-month vola, scaled by 6-month average</t>
+  </si>
+  <si>
+    <t>Inverse rolling 12-month vola, scaled by 3-month average</t>
+  </si>
+  <si>
+    <t>Sign of difference in 12-month average minus current volatility</t>
+  </si>
+  <si>
+    <t>mom1 scaled by 3Y past return volatility and annualized</t>
+  </si>
+  <si>
+    <t>mom3 scaled by 3Y past return volatility and annualized</t>
+  </si>
+  <si>
+    <t>mom6 scaled by 3Y past return volatility and annualized</t>
+  </si>
+  <si>
+    <t>rev1</t>
+  </si>
+  <si>
+    <t>rev2</t>
+  </si>
+  <si>
+    <t>rev3</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-3$ to $t$</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-6$ to $t$</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-12$ to $t$</t>
+  </si>
+  <si>
+    <t>Characteristic Spread</t>
+  </si>
+  <si>
+    <t>12-month z-score of the factor signal</t>
+  </si>
+  <si>
+    <t>char1</t>
+  </si>
+  <si>
+    <t>char2</t>
+  </si>
+  <si>
+    <t>char3</t>
+  </si>
+  <si>
+    <t>6-month z-score of the factor signal</t>
+  </si>
+  <si>
+    <t>3-month z-score of the factor signal</t>
   </si>
 </sst>
 </file>
@@ -763,8 +829,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}" name="Table4" displayName="Table4" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}" name="Table4" displayName="Table4" ref="A1:D19" totalsRowShown="0">
+  <autoFilter ref="A1:D19" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B3F054F8-43F3-4479-8D0E-B4E34DB18A84}" name="Acronym"/>
     <tableColumn id="2" xr3:uid="{899B32B6-D017-485C-B46D-6C38007B1277}" name="Category"/>
@@ -1727,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1752AB43-D4D0-4055-B83C-18A0D13E7988}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2247,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07290A6-0F3B-4D1A-8BCE-9248DD61F846}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2298,7 +2364,7 @@
         <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
@@ -2326,7 +2392,7 @@
         <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
@@ -2354,7 +2420,7 @@
         <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
@@ -2382,25 +2448,155 @@
         <v>128</v>
       </c>
       <c r="D9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21" customHeight="1">
+      <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1">
+      <c r="A12" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="21" customHeight="1"/>
-    <row r="11" spans="1:4" ht="21" customHeight="1"/>
-    <row r="12" spans="1:4" ht="21" customHeight="1"/>
-    <row r="13" spans="1:4" ht="21" customHeight="1"/>
-    <row r="14" spans="1:4" ht="21" customHeight="1"/>
-    <row r="15" spans="1:4" ht="21" customHeight="1"/>
-    <row r="16" spans="1:4" ht="21" customHeight="1"/>
-    <row r="17" ht="21" customHeight="1"/>
-    <row r="18" ht="21" customHeight="1"/>
-    <row r="19" ht="21" customHeight="1"/>
-    <row r="20" ht="21" customHeight="1"/>
-    <row r="21" ht="21" customHeight="1"/>
-    <row r="22" ht="21" customHeight="1"/>
-    <row r="23" ht="21" customHeight="1"/>
-    <row r="24" ht="21" customHeight="1"/>
-    <row r="25" ht="21" customHeight="1"/>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1">
+      <c r="A13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1">
+      <c r="A14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21" customHeight="1">
+      <c r="A15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1">
+      <c r="A16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21" customHeight="1">
+      <c r="A17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21" customHeight="1">
+      <c r="A18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21" customHeight="1">
+      <c r="A19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21" customHeight="1"/>
+    <row r="21" spans="1:4" ht="21" customHeight="1"/>
+    <row r="22" spans="1:4" ht="21" customHeight="1"/>
+    <row r="23" spans="1:4" ht="21" customHeight="1"/>
+    <row r="24" spans="1:4" ht="21" customHeight="1"/>
+    <row r="25" spans="1:4" ht="21" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Methodology for signal timing
</commit_message>
<xml_diff>
--- a/methodology.xlsx
+++ b/methodology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pertl\Desktop\timing_bond_factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3111C23F-F31E-4210-BC41-F4374E4B5C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21D1E9D-A4C4-4BF9-8D08-5E37418380E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="249">
   <si>
     <t>Name</t>
   </si>
@@ -634,70 +634,157 @@
     <t>vol3</t>
   </si>
   <si>
-    <t>vol4</t>
+    <t>Inverse rolling 12-month vola, scaled by 12-month average</t>
+  </si>
+  <si>
+    <t>Inverse rolling 12-month vola, scaled by 6-month average</t>
+  </si>
+  <si>
+    <t>Inverse rolling 12-month vola, scaled by 3-month average</t>
+  </si>
+  <si>
+    <t>mom1 scaled by 3Y past return volatility and annualized</t>
+  </si>
+  <si>
+    <t>mom3 scaled by 3Y past return volatility and annualized</t>
+  </si>
+  <si>
+    <t>mom6 scaled by 3Y past return volatility and annualized</t>
+  </si>
+  <si>
+    <t>rev1</t>
+  </si>
+  <si>
+    <t>rev2</t>
+  </si>
+  <si>
+    <t>rev3</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-3$ to $t$</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-6$ to $t$</t>
+  </si>
+  <si>
+    <t>1 minus annualized avg return over $t-12$ to $t$</t>
+  </si>
+  <si>
+    <t>Characteristic Spread</t>
+  </si>
+  <si>
+    <t>12-month z-score of the factor signal</t>
+  </si>
+  <si>
+    <t>char1</t>
+  </si>
+  <si>
+    <t>char2</t>
+  </si>
+  <si>
+    <t>char3</t>
+  </si>
+  <si>
+    <t>6-month z-score of the factor signal</t>
+  </si>
+  <si>
+    <t>3-month z-score of the factor signal</t>
+  </si>
+  <si>
+    <t>fed</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>cpi</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>tvix</t>
+  </si>
+  <si>
+    <t>vix</t>
+  </si>
+  <si>
+    <t>Federal Funds Rate</t>
+  </si>
+  <si>
+    <t>Real GDP Growth</t>
+  </si>
+  <si>
+    <t>CPI YOY Inflation</t>
+  </si>
+  <si>
+    <t>10y - fed funds</t>
+  </si>
+  <si>
+    <t>Treasury VIX</t>
+  </si>
+  <si>
+    <t>CBOE VIX</t>
   </si>
   <si>
     <t>Pertl (2025)</t>
   </si>
   <si>
-    <t>Inverse rolling 12-month vola, scaled by 12-month average</t>
-  </si>
-  <si>
-    <t>Inverse rolling 12-month vola, scaled by 6-month average</t>
-  </si>
-  <si>
-    <t>Inverse rolling 12-month vola, scaled by 3-month average</t>
-  </si>
-  <si>
-    <t>Sign of difference in 12-month average minus current volatility</t>
-  </si>
-  <si>
-    <t>mom1 scaled by 3Y past return volatility and annualized</t>
-  </si>
-  <si>
-    <t>mom3 scaled by 3Y past return volatility and annualized</t>
-  </si>
-  <si>
-    <t>mom6 scaled by 3Y past return volatility and annualized</t>
-  </si>
-  <si>
-    <t>rev1</t>
-  </si>
-  <si>
-    <t>rev2</t>
-  </si>
-  <si>
-    <t>rev3</t>
-  </si>
-  <si>
-    <t>1 minus annualized avg return over $t-3$ to $t$</t>
-  </si>
-  <si>
-    <t>1 minus annualized avg return over $t-6$ to $t$</t>
-  </si>
-  <si>
-    <t>1 minus annualized avg return over $t-12$ to $t$</t>
-  </si>
-  <si>
-    <t>Characteristic Spread</t>
-  </si>
-  <si>
-    <t>12-month z-score of the factor signal</t>
-  </si>
-  <si>
-    <t>char1</t>
-  </si>
-  <si>
-    <t>char2</t>
-  </si>
-  <si>
-    <t>char3</t>
-  </si>
-  <si>
-    <t>6-month z-score of the factor signal</t>
-  </si>
-  <si>
-    <t>3-month z-score of the factor signal</t>
+    <t>Rolling Beta of look-ahead return against signal, times current signal value. Scaled by 10 with baselevel 0.5</t>
+  </si>
+  <si>
+    <t>mom</t>
+  </si>
+  <si>
+    <t>vol</t>
+  </si>
+  <si>
+    <t>rev</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Overall Momentum</t>
+  </si>
+  <si>
+    <t>Overall Volatility</t>
+  </si>
+  <si>
+    <t>Overall Reversal</t>
+  </si>
+  <si>
+    <t>Overall Characteristic Spread</t>
+  </si>
+  <si>
+    <t>Overall Macro</t>
+  </si>
+  <si>
+    <t>Aggregation of all</t>
+  </si>
+  <si>
+    <t>Simple Mean of all momentum signals</t>
+  </si>
+  <si>
+    <t>Simple Mean of all volatility signals</t>
+  </si>
+  <si>
+    <t>Simple Mean of all reversal signals</t>
+  </si>
+  <si>
+    <t>Simple Mean of all characteristic spread signals</t>
+  </si>
+  <si>
+    <t>Simple Mean of all macro signals</t>
+  </si>
+  <si>
+    <t>Simple mean of all aggregated signals</t>
   </si>
 </sst>
 </file>
@@ -829,8 +916,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}" name="Table4" displayName="Table4" ref="A1:D19" totalsRowShown="0">
-  <autoFilter ref="A1:D19" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}" name="Table4" displayName="Table4" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30" xr:uid="{75E9DB02-444F-45D5-85E3-F729A403A2DB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B3F054F8-43F3-4479-8D0E-B4E34DB18A84}" name="Acronym"/>
     <tableColumn id="2" xr3:uid="{899B32B6-D017-485C-B46D-6C38007B1277}" name="Category"/>
@@ -2311,18 +2398,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07290A6-0F3B-4D1A-8BCE-9248DD61F846}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.21875" customWidth="1"/>
-    <col min="4" max="4" width="69.6640625" customWidth="1"/>
+    <col min="4" max="4" width="88.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
@@ -2364,7 +2451,7 @@
         <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
@@ -2392,7 +2479,7 @@
         <v>128</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1">
@@ -2420,7 +2507,7 @@
         <v>128</v>
       </c>
       <c r="D7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1">
@@ -2462,7 +2549,7 @@
         <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1">
@@ -2476,7 +2563,7 @@
         <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1">
@@ -2490,26 +2577,26 @@
         <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1">
       <c r="A14" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
         <v>112</v>
@@ -2518,12 +2605,12 @@
         <v>153</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B15" t="s">
         <v>112</v>
@@ -2532,49 +2619,49 @@
         <v>153</v>
       </c>
       <c r="D15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1">
       <c r="A16" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1">
       <c r="A17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B17" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C17" t="s">
         <v>168</v>
       </c>
       <c r="D17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21" customHeight="1">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>168</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="21" customHeight="1">
@@ -2582,21 +2669,169 @@
         <v>217</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
-        <v>168</v>
+        <v>229</v>
       </c>
       <c r="D19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21" customHeight="1">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21" customHeight="1">
+      <c r="A21" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="21" customHeight="1"/>
-    <row r="21" spans="1:4" ht="21" customHeight="1"/>
-    <row r="22" spans="1:4" ht="21" customHeight="1"/>
-    <row r="23" spans="1:4" ht="21" customHeight="1"/>
-    <row r="24" spans="1:4" ht="21" customHeight="1"/>
-    <row r="25" spans="1:4" ht="21" customHeight="1"/>
+      <c r="B21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="21" customHeight="1">
+      <c r="A22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1">
+      <c r="A23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21" customHeight="1">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D26" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C27" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" t="s">
+        <v>229</v>
+      </c>
+      <c r="D28" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>235</v>
+      </c>
+      <c r="B29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C29" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>236</v>
+      </c>
+      <c r="B30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" t="s">
+        <v>229</v>
+      </c>
+      <c r="D30" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>